<commit_message>
made 2019 bl sheet
</commit_message>
<xml_diff>
--- a/Queries/Bulk Liquid Specs.xlsx
+++ b/Queries/Bulk Liquid Specs.xlsx
@@ -8,20 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mat/Projects/PDI/noidle/Queries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB209ED-E213-FE49-A6EE-6CD33249AEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88CD6B8-4E22-A74E-A6CB-D205513EE12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bulk Liquid tests since 2019" sheetId="2" r:id="rId1"/>
+    <sheet name="BL_Product_spec" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bulk Liquid tests since 2019'!$A$1:$G$1362</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BL_Product_spec!$A$1:$G$1362</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1793,14 +1799,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="3" bestFit="1" customWidth="1"/>

</xml_diff>